<commit_message>
Small bug fix (col missing) and format added to photos
</commit_message>
<xml_diff>
--- a/GetADobjects/_Docs/AD Column map.xlsx
+++ b/GetADobjects/_Docs/AD Column map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\GetADobjects\GetADobjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\GetADobjects\GetADobjects\_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Computers!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Contacts!$A$1:$I$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Groups!$A$1:$I$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$I$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$I$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WellKnownSIDs!$A$1:$I$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="184">
   <si>
     <t>max_length</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t>nop</t>
+  </si>
+  <si>
+    <t>UserMustChangePasswordAtNextLogon</t>
   </si>
 </sst>
 </file>
@@ -919,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1024,7 @@
         <v>156</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H67" si="1">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
+        <f t="shared" ref="H3:H68" si="1">CONCATENATE("new TableColDef(""",C3,""", typeof(",B3,"), """,G3,""",""",F3,"""),")</f>
         <v>new TableColDef("Initials", typeof(String), "initials","Adprop"),</v>
       </c>
       <c r="I3" t="str">
@@ -1797,7 +1800,7 @@
         <v>new TableColDef("Enabled", typeof(Boolean), "ACCOUNTDISABLE","UAC"),</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" ref="I28:I50" si="2">CONCATENATE("[",C28,"] [",A28,"] ",E28,",")</f>
+        <f t="shared" ref="I28:I51" si="2">CONCATENATE("[",C28,"] [",A28,"] ",E28,",")</f>
         <v>[Enabled] [bit] NULL,</v>
       </c>
     </row>
@@ -2161,7 +2164,7 @@
         <v>new TableColDef("UseDESKeyOnly", typeof(Boolean), "USE_DES_KEY_ONLY","UAC"),</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="2"/>
+        <f>CONCATENATE("[",C41,"] [",A41,"] ",E42,",")</f>
         <v>[UseDESKeyOnly] [bit] NULL,</v>
       </c>
     </row>
@@ -2173,164 +2176,164 @@
         <v>72</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E42" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G42" t="s">
+        <v>181</v>
+      </c>
+      <c r="H42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>new TableColDef("UserMustChangePasswordAtNextLogon", typeof(Boolean), "does_not_exist_in_AD","nop"),</v>
+      </c>
+      <c r="I42" t="str">
+        <f>CONCATENATE("[",C42,"] [",A42,"] ",E43,",")</f>
+        <v>[UserMustChangePasswordAtNextLogon] [bit] NULL,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E42" t="s">
-        <v>96</v>
-      </c>
-      <c r="F42" s="5" t="s">
+      <c r="E43" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G43" t="s">
         <v>92</v>
       </c>
-      <c r="H42" s="1" t="str">
+      <c r="H43" s="1" t="str">
         <f t="shared" si="1"/>
         <v>new TableColDef("HomedirRequired", typeof(Boolean), "HOMEDIR_REQUIRED","UAC"),</v>
       </c>
-      <c r="I42" t="str">
+      <c r="I43" t="str">
         <f t="shared" si="2"/>
         <v>[HomedirRequired] [bit] NULL,</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>73</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>35</v>
       </c>
-      <c r="E43" t="s">
-        <v>96</v>
-      </c>
-      <c r="F43" s="5" t="s">
+      <c r="E44" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G44" t="s">
         <v>130</v>
       </c>
-      <c r="H43" s="1" t="str">
+      <c r="H44" s="1" t="str">
         <f t="shared" si="1"/>
         <v>new TableColDef("LastBadPasswordAttempt", typeof(DateTime), "badpasswordtime","filetime"),</v>
       </c>
-      <c r="I43" t="str">
+      <c r="I44" t="str">
         <f t="shared" si="2"/>
         <v>[LastBadPasswordAttempt] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>8</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>74</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>9</v>
       </c>
-      <c r="E44" t="s">
-        <v>96</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="E45" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G45" t="s">
         <v>124</v>
       </c>
-      <c r="H44" s="1" t="str">
+      <c r="H45" s="1" t="str">
         <f t="shared" si="1"/>
         <v>new TableColDef("BadLogonCount", typeof(Int32), "badpwdcount","Adprop"),</v>
       </c>
-      <c r="I44" t="str">
+      <c r="I45" t="str">
         <f t="shared" si="2"/>
         <v>[BadLogonCount] [int] NULL,</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>2</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>73</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>36</v>
       </c>
-      <c r="E45" t="s">
-        <v>96</v>
-      </c>
-      <c r="F45" s="5" t="s">
+      <c r="E46" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G46" t="s">
         <v>173</v>
       </c>
-      <c r="H45" s="1" t="str">
+      <c r="H46" s="1" t="str">
         <f t="shared" si="1"/>
         <v>new TableColDef("LastLogonDate", typeof(DateTime), "lastlogon","filetime"),</v>
       </c>
-      <c r="I45" t="str">
+      <c r="I46" t="str">
         <f t="shared" si="2"/>
         <v>[LastLogonDate] [datetime] NULL,</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>8</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E46" t="s">
-        <v>96</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="E47" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" t="s">
         <v>121</v>
       </c>
-      <c r="H46" s="1" t="str">
+      <c r="H47" s="1" t="str">
         <f t="shared" si="1"/>
         <v>new TableColDef("LogonCount", typeof(Int32), "logoncount","Adprop"),</v>
       </c>
-      <c r="I46" t="str">
+      <c r="I47" t="str">
         <f t="shared" si="2"/>
         <v>[LogonCount] [int] NULL,</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G47" t="s">
-        <v>123</v>
-      </c>
-      <c r="H47" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>new TableColDef("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime"),</v>
-      </c>
-      <c r="I47" t="str">
-        <f t="shared" si="2"/>
-        <v>[PasswordLastSet] [datetime] NULL,</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2341,7 +2344,7 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="E48" t="s">
         <v>96</v>
@@ -2350,15 +2353,15 @@
         <v>144</v>
       </c>
       <c r="G48" t="s">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="H48" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("PasswordExpiryTime", typeof(DateTime), "msDS-UserPasswordExpiryTimeComputed","filetime"),</v>
+        <v>new TableColDef("PasswordLastSet", typeof(DateTime), "pwdlastset","filetime"),</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="2"/>
-        <v>[PasswordExpiryTime] [datetime] NULL,</v>
+        <v>[PasswordLastSet] [datetime] NULL,</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2369,7 +2372,7 @@
         <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s">
         <v>96</v>
@@ -2378,15 +2381,15 @@
         <v>144</v>
       </c>
       <c r="G49" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="H49" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime"),</v>
+        <v>new TableColDef("PasswordExpiryTime", typeof(DateTime), "msDS-UserPasswordExpiryTimeComputed","filetime"),</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="2"/>
-        <v>[AccountLockoutTime] [datetime] NULL,</v>
+        <v>[PasswordExpiryTime] [datetime] NULL,</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2397,7 +2400,7 @@
         <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E50" t="s">
         <v>96</v>
@@ -2406,46 +2409,43 @@
         <v>144</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="H50" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime"),</v>
+        <v>new TableColDef("AccountLockoutTime", typeof(DateTime), "lockouttime","filetime"),</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="2"/>
-        <v>[AccountExpirationDate] [datetime] NULL,</v>
+        <v>[AccountLockoutTime] [datetime] NULL,</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51">
-        <v>128</v>
+        <v>73</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
       </c>
       <c r="E51" t="s">
         <v>96</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G51" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="H51" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("LogonWorkstations", typeof(String), "userworkstations","Adprop"),</v>
+        <v>new TableColDef("AccountExpirationDate", typeof(DateTime), "accountexpires","filetime"),</v>
       </c>
       <c r="I51" t="str">
-        <f>CONCATENATE("[",C51,"] [",A51,"](",D51,") ",E51,",")</f>
-        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
+        <f t="shared" si="2"/>
+        <v>[AccountExpirationDate] [datetime] NULL,</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>75</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D52">
         <v>128</v>
@@ -2468,15 +2468,15 @@
         <v>147</v>
       </c>
       <c r="G52" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H52" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("HomeDirectory", typeof(String), "homedirectory","Adprop"),</v>
+        <v>new TableColDef("LogonWorkstations", typeof(String), "userworkstations","Adprop"),</v>
       </c>
       <c r="I52" t="str">
         <f>CONCATENATE("[",C52,"] [",A52,"](",D52,") ",E52,",")</f>
-        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
+        <v>[LogonWorkstations] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2487,10 +2487,10 @@
         <v>75</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D53">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E53" t="s">
         <v>96</v>
@@ -2499,15 +2499,15 @@
         <v>147</v>
       </c>
       <c r="G53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H53" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("HomeDrive", typeof(String), "homedrive","Adprop"),</v>
+        <v>new TableColDef("HomeDirectory", typeof(String), "homedirectory","Adprop"),</v>
       </c>
       <c r="I53" t="str">
         <f>CONCATENATE("[",C53,"] [",A53,"](",D53,") ",E53,",")</f>
-        <v>[HomeDrive] [nvarchar](64) NULL,</v>
+        <v>[HomeDirectory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2517,11 +2517,11 @@
       <c r="B54" t="s">
         <v>75</v>
       </c>
-      <c r="C54" t="s">
-        <v>56</v>
+      <c r="C54" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D54">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E54" t="s">
         <v>96</v>
@@ -2530,15 +2530,15 @@
         <v>147</v>
       </c>
       <c r="G54" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H54" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ProfilePath", typeof(String), "profilepath","Adprop"),</v>
+        <v>new TableColDef("HomeDrive", typeof(String), "homedrive","Adprop"),</v>
       </c>
       <c r="I54" t="str">
         <f>CONCATENATE("[",C54,"] [",A54,"](",D54,") ",E54,",")</f>
-        <v>[ProfilePath] [nvarchar](128) NULL,</v>
+        <v>[HomeDrive] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2549,10 +2549,10 @@
         <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D55">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E55" t="s">
         <v>96</v>
@@ -2561,26 +2561,29 @@
         <v>147</v>
       </c>
       <c r="G55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H55" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ScriptPath", typeof(String), "scriptpath","Adprop"),</v>
+        <v>new TableColDef("ProfilePath", typeof(String), "profilepath","Adprop"),</v>
       </c>
       <c r="I55" t="str">
         <f>CONCATENATE("[",C55,"] [",A55,"](",D55,") ",E55,",")</f>
-        <v>[ScriptPath] [nvarchar](256) NULL,</v>
+        <v>[ProfilePath] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>85</v>
+        <v>58</v>
+      </c>
+      <c r="D56">
+        <v>256</v>
       </c>
       <c r="E56" t="s">
         <v>96</v>
@@ -2589,15 +2592,15 @@
         <v>147</v>
       </c>
       <c r="G56" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop"),</v>
+        <v>new TableColDef("ScriptPath", typeof(String), "scriptpath","Adprop"),</v>
       </c>
       <c r="I56" t="str">
-        <f>CONCATENATE("[",C56,"] [",A56,"] ",E56,",")</f>
-        <v>[userAccountControl] [int] NULL,</v>
+        <f>CONCATENATE("[",C56,"] [",A56,"](",D56,") ",E56,",")</f>
+        <v>[ScriptPath] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2607,11 +2610,8 @@
       <c r="B57" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57">
-        <v>128</v>
+      <c r="C57" t="s">
+        <v>85</v>
       </c>
       <c r="E57" t="s">
         <v>96</v>
@@ -2620,29 +2620,29 @@
         <v>147</v>
       </c>
       <c r="G57" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H57" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop"),</v>
+        <v>new TableColDef("userAccountControl", typeof(Int32), "useraccountcontrol","Adprop"),</v>
       </c>
       <c r="I57" t="str">
         <f>CONCATENATE("[",C57,"] [",A57,"] ",E57,",")</f>
-        <v>[PrimaryGroupID] [int] NULL,</v>
+        <v>[userAccountControl] [int] NULL,</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" t="s">
-        <v>43</v>
+        <v>74</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="D58">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
         <v>96</v>
@@ -2651,15 +2651,15 @@
         <v>147</v>
       </c>
       <c r="G58" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="H58" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
+        <v>new TableColDef("PrimaryGroupID", typeof(Int32), "primarygroupid","Adprop"),</v>
       </c>
       <c r="I58" t="str">
-        <f>CONCATENATE("[",C58,"] [",A58,"](",D58,") ",E58,",")</f>
-        <v>[Name] [nvarchar](256) NULL,</v>
+        <f>CONCATENATE("[",C58,"] [",A58,"] ",E58,",")</f>
+        <v>[PrimaryGroupID] [int] NULL,</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D59">
         <v>256</v>
@@ -2682,15 +2682,15 @@
         <v>147</v>
       </c>
       <c r="G59" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="H59" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("CN", typeof(String), "cn","Adprop"),</v>
+        <v>new TableColDef("Name", typeof(String), "name","Adprop"),</v>
       </c>
       <c r="I59" t="str">
         <f>CONCATENATE("[",C59,"] [",A59,"](",D59,") ",E59,",")</f>
-        <v>[CN] [nvarchar](256) NULL,</v>
+        <v>[Name] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2701,7 +2701,7 @@
         <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D60">
         <v>256</v>
@@ -2713,15 +2713,15 @@
         <v>147</v>
       </c>
       <c r="G60" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="H60" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("UserPrincipalName", typeof(String), "userprincipalname","Adprop"),</v>
+        <v>new TableColDef("CN", typeof(String), "cn","Adprop"),</v>
       </c>
       <c r="I60" t="str">
         <f>CONCATENATE("[",C60,"] [",A60,"](",D60,") ",E60,",")</f>
-        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
+        <v>[CN] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2732,10 +2732,10 @@
         <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D61">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="E61" t="s">
         <v>96</v>
@@ -2744,15 +2744,15 @@
         <v>147</v>
       </c>
       <c r="G61" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="H61" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("SamAccountName", typeof(String), "samaccountname","Adprop"),</v>
+        <v>new TableColDef("UserPrincipalName", typeof(String), "userprincipalname","Adprop"),</v>
       </c>
       <c r="I61" t="str">
         <f>CONCATENATE("[",C61,"] [",A61,"](",D61,") ",E61,",")</f>
-        <v>[SamAccountName] [nvarchar](128) NULL,</v>
+        <v>[UserPrincipalName] [nvarchar](256) NULL,</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2763,10 +2763,10 @@
         <v>75</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="D62">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="E62" t="s">
         <v>96</v>
@@ -2775,26 +2775,29 @@
         <v>147</v>
       </c>
       <c r="G62" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H62" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
+        <v>new TableColDef("SamAccountName", typeof(String), "samaccountname","Adprop"),</v>
       </c>
       <c r="I62" t="str">
         <f>CONCATENATE("[",C62,"] [",A62,"](",D62,") ",E62,",")</f>
-        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
+        <v>[SamAccountName] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>16</v>
+        <v>75</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63">
+        <v>512</v>
       </c>
       <c r="E63" t="s">
         <v>96</v>
@@ -2803,15 +2806,15 @@
         <v>147</v>
       </c>
       <c r="G63" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="H63" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("Created", typeof(DateTime), "whencreated","Adprop"),</v>
+        <v>new TableColDef("DistinguishedName", typeof(String), "distinguishedname","Adprop"),</v>
       </c>
       <c r="I63" t="str">
-        <f>CONCATENATE("[",C63,"] [",A63,"] ",E63,",")</f>
-        <v>[Created] [datetime] NULL,</v>
+        <f>CONCATENATE("[",C63,"] [",A63,"](",D63,") ",E63,",")</f>
+        <v>[DistinguishedName] [nvarchar](512) NULL,</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2822,7 +2825,7 @@
         <v>73</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E64" t="s">
         <v>96</v>
@@ -2831,29 +2834,26 @@
         <v>147</v>
       </c>
       <c r="G64" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H64" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("Modified", typeof(DateTime), "whenchanged","Adprop"),</v>
+        <v>new TableColDef("Created", typeof(DateTime), "whencreated","Adprop"),</v>
       </c>
       <c r="I64" t="str">
         <f>CONCATENATE("[",C64,"] [",A64,"] ",E64,",")</f>
-        <v>[Modified] [datetime] NULL,</v>
+        <v>[Created] [datetime] NULL,</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>44</v>
-      </c>
-      <c r="D65">
-        <v>128</v>
+        <v>73</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E65" t="s">
         <v>96</v>
@@ -2862,15 +2862,15 @@
         <v>147</v>
       </c>
       <c r="G65" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="H65" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
+        <v>new TableColDef("Modified", typeof(DateTime), "whenchanged","Adprop"),</v>
       </c>
       <c r="I65" t="str">
-        <f>CONCATENATE("[",C65,"] [",A65,"](",D65,") ",E65,",")</f>
-        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
+        <f>CONCATENATE("[",C65,"] [",A65,"] ",E65,",")</f>
+        <v>[Modified] [datetime] NULL,</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,27 +2881,27 @@
         <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D66">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
         <v>96</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G66" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H66" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
+        <v>new TableColDef("ObjectCategory", typeof(String), "objectcategory","Adprop"),</v>
       </c>
       <c r="I66" t="str">
         <f>CONCATENATE("[",C66,"] [",A66,"](",D66,") ",E66,",")</f>
-        <v>[ObjectClass] [nvarchar](64) NULL,</v>
+        <v>[ObjectCategory] [nvarchar](128) NULL,</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2912,55 +2912,58 @@
         <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D67">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="E67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="G67" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H67" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>new TableColDef("SID", typeof(String), "objectsid","SID"),</v>
+        <v>new TableColDef("ObjectClass", typeof(String), "SchemaClassName","ObjClass"),</v>
       </c>
       <c r="I67" t="str">
         <f>CONCATENATE("[",C67,"] [",A67,"](",D67,") ",E67,",")</f>
-        <v>[SID] [nvarchar](128) NOT NULL,</v>
+        <v>[ObjectClass] [nvarchar](64) NULL,</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D68">
+        <v>128</v>
       </c>
       <c r="E68" t="s">
         <v>97</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>146</v>
+        <v>59</v>
       </c>
       <c r="G68" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f t="shared" ref="H68:H69" si="3">CONCATENATE("new TableColDef(""",C68,""", typeof(",B68,"), """,G68,""",""",F68,"""),")</f>
-        <v>new TableColDef("ObjectGUID", typeof(Guid), "Guid","ObjGuid"),</v>
+        <f t="shared" si="1"/>
+        <v>new TableColDef("SID", typeof(String), "objectsid","SID"),</v>
       </c>
       <c r="I68" t="str">
-        <f>CONCATENATE("[",C68,"] [",A68,"] ",E68,",")</f>
-        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
+        <f>CONCATENATE("[",C68,"] [",A68,"](",D68,") ",E68,",")</f>
+        <v>[SID] [nvarchar](128) NOT NULL,</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2971,28 +2974,56 @@
         <v>70</v>
       </c>
       <c r="C69" t="s">
+        <v>47</v>
+      </c>
+      <c r="E69" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G69" t="s">
+        <v>70</v>
+      </c>
+      <c r="H69" s="1" t="str">
+        <f t="shared" ref="H69:H70" si="3">CONCATENATE("new TableColDef(""",C69,""", typeof(",B69,"), """,G69,""",""",F69,"""),")</f>
+        <v>new TableColDef("ObjectGUID", typeof(Guid), "Guid","ObjGuid"),</v>
+      </c>
+      <c r="I69" t="str">
+        <f>CONCATENATE("[",C69,"] [",A69,"] ",E69,",")</f>
+        <v>[ObjectGUID] [uniqueidentifier] NOT NULL,</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" t="s">
         <v>180</v>
       </c>
-      <c r="E69" t="s">
-        <v>96</v>
-      </c>
-      <c r="F69" s="5" t="s">
+      <c r="E70" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G70" t="s">
         <v>181</v>
       </c>
-      <c r="H69" s="1" t="str">
+      <c r="H70" s="1" t="str">
         <f t="shared" si="3"/>
         <v>new TableColDef("ManagerGUID", typeof(Guid), "does_not_exist_in_AD","nop"),</v>
       </c>
-      <c r="I69" t="str">
-        <f>CONCATENATE("[",C69,"] [",A69,"] ",E69,",")</f>
+      <c r="I70" t="str">
+        <f>CONCATENATE("[",C70,"] [",A70,"] ",E70,",")</f>
         <v>[ManagerGUID] [uniqueidentifier] NULL,</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I61"/>
+  <autoFilter ref="A1:I62"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>